<commit_message>
Created pairwise Sankey plots
</commit_message>
<xml_diff>
--- a/asctb_mapper/Azimuth_CellTypist_PopV_Lung_ASCTB_Crosswalks.xlsx
+++ b/asctb_mapper/Azimuth_CellTypist_PopV_Lung_ASCTB_Crosswalks.xlsx
@@ -5,23 +5,25 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Vikrant\Github_Repositories\scRNA-seq-papers-and-analyses\Vikrant_Analyses\ASCTB_Mapper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Vikrant\Github_Repositories\ct-ann-predictive-analytics\asctb_mapper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C624EEE3-51EC-4213-A195-F1741845CF23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B153C4B-D619-4900-94B7-B272B08A2321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="641" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="641" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Azimuth-HLCAv2Labels_to_ASCTBLa" sheetId="1" r:id="rId1"/>
     <sheet name="Closest (manual) crosswalk" sheetId="4" r:id="rId2"/>
     <sheet name="Cleaner_manual_crosswalk" sheetId="2" r:id="rId3"/>
     <sheet name="Collating_Glorias_Feedback" sheetId="6" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Azimuth-HLCAv2Labels_to_ASCTBLa'!$A$1:$L$90</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Cleaner_manual_crosswalk!$A$1:$C$96</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Collating_Glorias_Feedback!$A$2:$N$128</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Sheet1!$A$1:$B$93</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -152,7 +154,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2622" uniqueCount="548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2789" uniqueCount="548">
   <si>
     <t>source</t>
   </si>
@@ -2470,18 +2472,6 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="44" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2498,6 +2488,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="44" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2545,7 +2547,47 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -7914,8 +7956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25971A9B-58AA-4348-A339-82E43E36C7DE}">
   <dimension ref="A1:N138"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView topLeftCell="A128" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7937,72 +7979,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="31" t="s">
         <v>543</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="23" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="28" t="s">
         <v>536</v>
       </c>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="24" t="s">
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="29" t="s">
         <v>537</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="25" t="s">
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="30" t="s">
         <v>538</v>
       </c>
-      <c r="M1" s="25"/>
-      <c r="N1" s="26" t="s">
+      <c r="M1" s="30"/>
+      <c r="N1" s="22" t="s">
         <v>546</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="23" t="s">
         <v>452</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="23" t="s">
         <v>453</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="28" t="s">
+      <c r="G2" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="29" t="s">
+      <c r="H2" s="25" t="s">
         <v>539</v>
       </c>
-      <c r="I2" s="29" t="s">
+      <c r="I2" s="25" t="s">
         <v>540</v>
       </c>
-      <c r="J2" s="29" t="s">
+      <c r="J2" s="25" t="s">
         <v>541</v>
       </c>
-      <c r="K2" s="29" t="s">
+      <c r="K2" s="25" t="s">
         <v>542</v>
       </c>
-      <c r="L2" s="30" t="s">
+      <c r="L2" s="26" t="s">
         <v>544</v>
       </c>
-      <c r="M2" s="30" t="s">
+      <c r="M2" s="26" t="s">
         <v>545</v>
       </c>
-      <c r="N2" s="31" t="s">
+      <c r="N2" s="27" t="s">
         <v>547</v>
       </c>
     </row>
@@ -13638,9 +13680,710 @@
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <conditionalFormatting sqref="B2 B115:B128">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FF100EF-9871-4F24-86C5-BB92AC616A94}">
+  <dimension ref="A1:B93"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>452</v>
+      </c>
+      <c r="B1" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>455</v>
+      </c>
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B13" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>106</v>
+      </c>
+      <c r="B14" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>130</v>
+      </c>
+      <c r="B16" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>135</v>
+      </c>
+      <c r="B17" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>143</v>
+      </c>
+      <c r="B18" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>151</v>
+      </c>
+      <c r="B19" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>155</v>
+      </c>
+      <c r="B20" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>161</v>
+      </c>
+      <c r="B21" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>174</v>
+      </c>
+      <c r="B22" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>180</v>
+      </c>
+      <c r="B23" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>182</v>
+      </c>
+      <c r="B24" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>208</v>
+      </c>
+      <c r="B26" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>458</v>
+      </c>
+      <c r="B28" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>229</v>
+      </c>
+      <c r="B29" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>246</v>
+      </c>
+      <c r="B30" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>262</v>
+      </c>
+      <c r="B32" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>268</v>
+      </c>
+      <c r="B33" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>284</v>
+      </c>
+      <c r="B35" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>290</v>
+      </c>
+      <c r="B36" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>297</v>
+      </c>
+      <c r="B37" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>300</v>
+      </c>
+      <c r="B38" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>308</v>
+      </c>
+      <c r="B39" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>462</v>
+      </c>
+      <c r="B40" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>319</v>
+      </c>
+      <c r="B42" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>325</v>
+      </c>
+      <c r="B43" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>329</v>
+      </c>
+      <c r="B44" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>343</v>
+      </c>
+      <c r="B45" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>348</v>
+      </c>
+      <c r="B46" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>354</v>
+      </c>
+      <c r="B47" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>361</v>
+      </c>
+      <c r="B48" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>374</v>
+      </c>
+      <c r="B50" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>382</v>
+      </c>
+      <c r="B53" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>468</v>
+      </c>
+      <c r="B54" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>469</v>
+      </c>
+      <c r="B55" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>470</v>
+      </c>
+      <c r="B56" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>361</v>
+      </c>
+      <c r="B58" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>67</v>
+      </c>
+      <c r="B60" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>22</v>
+      </c>
+      <c r="B61" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>477</v>
+      </c>
+      <c r="B64" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>483</v>
+      </c>
+      <c r="B65" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>484</v>
+      </c>
+      <c r="B66" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>486</v>
+      </c>
+      <c r="B67" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>107</v>
+      </c>
+      <c r="B68" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>117</v>
+      </c>
+      <c r="B69" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>493</v>
+      </c>
+      <c r="B72" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>494</v>
+      </c>
+      <c r="B73" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>192</v>
+      </c>
+      <c r="B74" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>496</v>
+      </c>
+      <c r="B76" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>501</v>
+      </c>
+      <c r="B77" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>253</v>
+      </c>
+      <c r="B78" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>502</v>
+      </c>
+      <c r="B79" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>265</v>
+      </c>
+      <c r="B80" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>133</v>
+      </c>
+      <c r="B81" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>112</v>
+      </c>
+      <c r="B82" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>507</v>
+      </c>
+      <c r="B83" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>70</v>
+      </c>
+      <c r="B84" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>146</v>
+      </c>
+      <c r="B85" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>232</v>
+      </c>
+      <c r="B86" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>508</v>
+      </c>
+      <c r="B87" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>509</v>
+      </c>
+      <c r="B88" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>510</v>
+      </c>
+      <c r="B89" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>514</v>
+      </c>
+      <c r="B90" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>516</v>
+      </c>
+      <c r="B91" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>518</v>
+      </c>
+      <c r="B92" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>519</v>
+      </c>
+      <c r="B93" t="s">
+        <v>178</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:B93" xr:uid="{8FF100EF-9871-4F24-86C5-BB92AC616A94}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>